<commit_message>
added screenshot of timings for programs and excel spreadsheet.
</commit_message>
<xml_diff>
--- a/Parallel/timings for nqueens.xlsx
+++ b/Parallel/timings for nqueens.xlsx
@@ -5,31 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mauleenndlovu/Desktop/Spring 2021/Concurrent Programming/HPC Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mauleenndlovu/Desktop/Spring 2021/Concurrent Programming/HPC Project/Ndlovu - HPC Project, N-Queens/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5283875D-356D-114B-A053-3A4AD9A7393F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195C5637-45D4-0A4C-AF15-99419AC9AEB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="520" windowWidth="34100" windowHeight="19560" xr2:uid="{91720354-27F5-544E-8A80-9F9BA77F37C6}"/>
+    <workbookView xWindow="2520" yWindow="700" windowWidth="30520" windowHeight="19560" xr2:uid="{91720354-27F5-544E-8A80-9F9BA77F37C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$2:$A$14</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$D$2:$D$14</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$2:$C$14</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$D$2:$D$14</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$A$2:$A$14</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$C$2:$C$14</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">N </t>
   </si>
@@ -61,12 +47,18 @@
   <si>
     <t>Number of Solutions</t>
   </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Speedup</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -80,13 +72,76 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -98,10 +153,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -109,8 +168,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="40% - Accent3" xfId="2" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="1" builtinId="36"/>
+    <cellStyle name="60% - Accent3" xfId="3" builtinId="40"/>
+    <cellStyle name="60% - Accent4" xfId="4" builtinId="44"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -246,10 +333,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$14</c:f>
+              <c:f>Sheet1!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -288,16 +375,19 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$14</c:f>
+              <c:f>Sheet1!$D$2:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>4.808E-5</c:v>
                 </c:pt>
@@ -336,6 +426,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>178.949197486</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1317.146654811</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -386,59 +479,64 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+            <c:strRef>
+              <c:f>Sheet1!$A$1:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>N </c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>9</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>15</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$14</c:f>
+              <c:f>Sheet1!$C$2:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>2.4665199999999998E-4</c:v>
                 </c:pt>
@@ -477,6 +575,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>153.66863675299999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1315.21475369</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -503,7 +604,7 @@
         <c:axId val="746193664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="15"/>
+          <c:max val="16"/>
           <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -609,7 +710,7 @@
         <c:axId val="746195312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="180"/>
+          <c:max val="1500"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -708,7 +809,7 @@
         <c:crossAx val="746193664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="10"/>
+        <c:majorUnit val="70"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -726,8 +827,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.43295672500022675"/>
           <c:y val="0.92706181770237994"/>
-          <c:w val="0.23843694942027019"/>
-          <c:h val="5.0989472110982516E-2"/>
+          <c:w val="0.23566306929025174"/>
+          <c:h val="4.8511146251646077E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -761,6 +862,489 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Speedup Graph</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> for N-Queens Problem</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Speedup</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$22:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$22:$D$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.19493050938163892</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21462528268836087</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.39002533272009166</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.37232729663808656</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0230517270125323</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1433318748632686</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1445458584363946</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2475795764010629</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2116243298285752</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.2403052035060185</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1982343455497382</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.18430300139495</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.164513470459394</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.0014688864427499</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-80DF-614C-9810-1AED94E38E9B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1805316255"/>
+        <c:axId val="1805209935"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1805316255"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>N</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1805209935"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1805209935"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Speed Up</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.0000" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1805316255"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -836,6 +1420,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1333,6 +1957,522 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1357,15 +2497,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>40538</xdr:colOff>
+      <xdr:colOff>30989</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>15169</xdr:rowOff>
+      <xdr:rowOff>19097</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>707527</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>19419</xdr:rowOff>
+      <xdr:colOff>263585</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>71887</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1385,6 +2525,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>10504</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>173062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>311509</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>107830</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08DD1AC7-8BAE-B149-A26F-1EE66B638DB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1690,30 +2866,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26DFD566-011B-4346-915C-700D8DFA7809}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="141" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="Q32" sqref="Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1890,7 +3068,7 @@
         <v>15</v>
       </c>
       <c r="B14" s="1">
-        <v>365596</v>
+        <v>2279184</v>
       </c>
       <c r="C14" s="2">
         <v>153.66863675299999</v>
@@ -1899,28 +3077,152 @@
         <v>178.949197486</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>16</v>
       </c>
-      <c r="B22">
+      <c r="B15" s="2">
         <v>14772512</v>
       </c>
+      <c r="C15" s="2">
+        <v>1315.21475369</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1317.146654811</v>
+      </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>17</v>
-      </c>
-      <c r="B23">
-        <v>95815104</v>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C21" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>18</v>
-      </c>
-      <c r="B24">
-        <v>666090624</v>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C22" s="9">
+        <v>1</v>
+      </c>
+      <c r="D22" s="10">
+        <f>D2/C2</f>
+        <v>0.19493050938163892</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C23" s="9">
+        <v>4</v>
+      </c>
+      <c r="D23" s="10">
+        <f>D3/C3</f>
+        <v>0.21462528268836087</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C24" s="9">
+        <v>5</v>
+      </c>
+      <c r="D24" s="10">
+        <f>D4/C4</f>
+        <v>0.39002533272009166</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C25" s="9">
+        <v>6</v>
+      </c>
+      <c r="D25" s="10">
+        <f>D5/C5</f>
+        <v>0.37232729663808656</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C26" s="9">
+        <v>7</v>
+      </c>
+      <c r="D26" s="10">
+        <f>D6/C6</f>
+        <v>1.0230517270125323</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C27" s="9">
+        <v>8</v>
+      </c>
+      <c r="D27" s="10">
+        <f>D7/C7</f>
+        <v>1.1433318748632686</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C28" s="9">
+        <v>9</v>
+      </c>
+      <c r="D28" s="10">
+        <f>D8/C8</f>
+        <v>1.1445458584363946</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C29" s="9">
+        <v>10</v>
+      </c>
+      <c r="D29" s="10">
+        <f>D9/C9</f>
+        <v>1.2475795764010629</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C30" s="9">
+        <v>11</v>
+      </c>
+      <c r="D30" s="10">
+        <f>D10/C10</f>
+        <v>1.2116243298285752</v>
+      </c>
+    </row>
+    <row r="31" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C31" s="9">
+        <v>12</v>
+      </c>
+      <c r="D31" s="10">
+        <f>D11/C11</f>
+        <v>1.2403052035060185</v>
+      </c>
+    </row>
+    <row r="32" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C32" s="9">
+        <v>13</v>
+      </c>
+      <c r="D32" s="10">
+        <f>D12/C12</f>
+        <v>1.1982343455497382</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C33" s="9">
+        <v>14</v>
+      </c>
+      <c r="D33" s="10">
+        <f>D13/C13</f>
+        <v>1.18430300139495</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C34" s="9">
+        <v>15</v>
+      </c>
+      <c r="D34" s="10">
+        <f>D14/C14</f>
+        <v>1.164513470459394</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C35" s="9">
+        <v>16</v>
+      </c>
+      <c r="D35" s="10">
+        <f>D15/C15</f>
+        <v>1.0014688864427499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>